<commit_message>
Started working towards quantum defect plot
</commit_message>
<xml_diff>
--- a/appendices/sr_data/rydberg_lines/compiled_rydberg_lines.xlsx
+++ b/appendices/sr_data/rydberg_lines/compiled_rydberg_lines.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F0EE3-5B5E-4583-8BB2-DB3F95DE62B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15870" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="5sns_1S0" sheetId="1" r:id="rId1"/>
+    <sheet name="5sns_3S1" sheetId="2" r:id="rId2"/>
+    <sheet name="5snd_1D2" sheetId="3" r:id="rId3"/>
+    <sheet name="5snd_3D1" sheetId="4" r:id="rId4"/>
+    <sheet name="5snd_3D2" sheetId="5" r:id="rId5"/>
+    <sheet name="5sns_3D3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,12 +336,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAB71F0-C9D0-4A36-9A78-2EC4E0BB2218}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953B5AE0-1549-4360-BBB0-59C7BECF3172}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9AD3DFA-CAD1-44E6-B59A-973C57F972B1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF4529D-212B-4392-8D1B-A97EC8A02B01}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60582CCF-64F9-42AA-9EB5-650B18D88714}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>